<commit_message>
added example dataset for Jerry's reference
</commit_message>
<xml_diff>
--- a/Data/Initial_Database.xlsx
+++ b/Data/Initial_Database.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhang\Documents\GitHub\Methane_Prediction\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry\Documents\GitHub\Methane_Prediction\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B99AC4E-4D63-492B-817C-1A08564175E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>Paper_Title</t>
   </si>
@@ -55,18 +56,43 @@
   </si>
   <si>
     <t>Cumulative_seaonal_CH4_kgCH4ha</t>
+  </si>
+  <si>
+    <t>130-140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M206</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">218-300 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions altered by the introduction of a year-long fallow to continuous rice systems</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/jeq2.70055</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -94,7 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -371,22 +397,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" customWidth="1"/>
+    <col min="7" max="7" width="32.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -412,23 +438,239 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>2021</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>2021</v>
+      </c>
+      <c r="G3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>2021</v>
+      </c>
+      <c r="G4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>2021</v>
+      </c>
+      <c r="G5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>2021</v>
+      </c>
+      <c r="G6">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>2021</v>
+      </c>
+      <c r="G7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>2021</v>
+      </c>
+      <c r="G8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>6000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>2021</v>
+      </c>
+      <c r="G9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>2021</v>
+      </c>
+      <c r="G10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>2021</v>
+      </c>
+      <c r="G11">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>2021</v>
+      </c>
+      <c r="G12">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>2021</v>
+      </c>
+      <c r="G13">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>2021</v>
+      </c>
+      <c r="G14">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>2021</v>
+      </c>
+      <c r="G15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>2021</v>
+      </c>
+      <c r="G16">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>2022</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="109.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -442,7 +684,19 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>